<commit_message>
extend Wrap aircraft fleet A319 and 320 neo
</commit_message>
<xml_diff>
--- a/airline/management/commands/AirlineFleet/AirlineFleet.xlsx
+++ b/airline/management/commands/AirlineFleet/AirlineFleet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\git\flight-profile\airline\management\commands\AirlineFleet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9496A0CF-E1C3-4610-83B3-B0AC01027032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E984F8DF-CA2B-49EA-9998-29861CAB6CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
   <si>
     <t>Aircraft</t>
   </si>
@@ -131,12 +131,39 @@
   <si>
     <t>TurnAround Time Minutes</t>
   </si>
+  <si>
+    <t>Airbus A319</t>
+  </si>
+  <si>
+    <t>Aircraft ICAO</t>
+  </si>
+  <si>
+    <t>A320</t>
+  </si>
+  <si>
+    <t>A319</t>
+  </si>
+  <si>
+    <t>A332</t>
+  </si>
+  <si>
+    <t>B738</t>
+  </si>
+  <si>
+    <t>B739</t>
+  </si>
+  <si>
+    <t>A20N</t>
+  </si>
+  <si>
+    <t>Airbus A320neo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +199,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -193,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -294,12 +327,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -372,6 +429,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -392,9 +470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -432,7 +510,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -538,7 +616,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -680,7 +758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -688,685 +766,931 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="16" customWidth="1"/>
-    <col min="11" max="13" width="17.453125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="35.1796875" customWidth="1"/>
-    <col min="16" max="256" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="16" customWidth="1"/>
+    <col min="12" max="14" width="17.453125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="35.1796875" customWidth="1"/>
+    <col min="17" max="257" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14">
+      <c r="D2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
         <v>16</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5">
         <v>18</v>
       </c>
-      <c r="I2" s="5">
+      <c r="J2" s="5">
         <v>123</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="14">
         <v>157</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>2890</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>1657</v>
       </c>
-      <c r="M2" s="5">
-        <v>25</v>
-      </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="5">
+        <v>25</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="14">
+      <c r="D3" s="14">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="14">
+      <c r="J3" s="5"/>
+      <c r="K3" s="14">
         <v>157</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
         <v>2840</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>1657</v>
       </c>
-      <c r="M3" s="5">
-        <v>25</v>
-      </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N3" s="5">
+        <v>25</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18">
+      <c r="D4" s="18">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>34</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="5">
+      <c r="G4" s="9"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="5">
         <v>32</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>168</v>
       </c>
-      <c r="J4" s="14">
+      <c r="K4" s="14">
         <v>234</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>3300</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>1857</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>35</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14">
+      <c r="D5" s="14">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
         <v>16</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
         <v>36</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="5">
         <v>108</v>
       </c>
-      <c r="J5" s="14">
+      <c r="K5" s="14">
         <v>160</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>3010</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>1557</v>
       </c>
-      <c r="M5" s="5">
-        <v>25</v>
-      </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="5">
+        <v>25</v>
+      </c>
+      <c r="O5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14">
+      <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>29</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
         <v>20</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
         <v>21</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>139</v>
       </c>
-      <c r="J6" s="15">
+      <c r="K6" s="15">
         <v>180</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <v>3050</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>1557</v>
       </c>
-      <c r="M6" s="6">
-        <v>25</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="6">
+        <v>25</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="18">
+        <v>5</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="15">
+        <v>150</v>
+      </c>
+      <c r="L7" s="6">
+        <v>2780</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1457</v>
+      </c>
+      <c r="N7" s="6">
+        <v>25</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="18">
+        <v>5</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="15">
+        <v>180</v>
+      </c>
+      <c r="L8" s="6">
+        <v>2780</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1457</v>
+      </c>
+      <c r="N8" s="6">
+        <v>25</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="18">
+      <c r="D9" s="18">
         <v>6</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5">
+      <c r="E9" s="26"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
         <v>16</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5">
         <v>18</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J9" s="5">
         <v>123</v>
       </c>
-      <c r="J7" s="14">
+      <c r="K9" s="14">
         <v>157</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L9" s="5">
         <v>2890</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M9" s="5">
         <v>1607</v>
       </c>
-      <c r="M7" s="5">
-        <v>25</v>
-      </c>
-      <c r="N7" s="10" t="s">
+      <c r="N9" s="5">
+        <v>25</v>
+      </c>
+      <c r="O9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="14">
+      <c r="D10" s="14">
         <v>7</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="14">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="14">
         <v>157</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L10" s="5">
         <v>2840</v>
       </c>
-      <c r="L8" s="5">
+      <c r="M10" s="5">
         <v>1607</v>
       </c>
-      <c r="M8" s="5">
-        <v>25</v>
-      </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="N10" s="5">
+        <v>25</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="14">
+      <c r="D11" s="14">
         <v>8</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9">
         <v>34</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="5">
+      <c r="G11" s="9"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="5">
         <v>32</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J11" s="5">
         <v>168</v>
       </c>
-      <c r="J9" s="14">
+      <c r="K11" s="14">
         <v>234</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L11" s="5">
         <v>3300</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M11" s="5">
         <v>1807</v>
       </c>
-      <c r="M9" s="5">
+      <c r="N11" s="5">
         <v>35</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="O11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="P11" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="18">
+      <c r="D12" s="18">
         <v>9</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
         <v>16</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5">
         <v>36</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J12" s="5">
         <v>108</v>
       </c>
-      <c r="J10" s="14">
+      <c r="K12" s="14">
         <v>160</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L12" s="5">
         <v>3010</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M12" s="5">
         <v>1507</v>
       </c>
-      <c r="M10" s="5">
-        <v>25</v>
-      </c>
-      <c r="N10" s="10" t="s">
+      <c r="N12" s="5">
+        <v>25</v>
+      </c>
+      <c r="O12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="P12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="14">
+      <c r="D13" s="14">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E13" s="7">
         <v>29</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
         <v>20</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
         <v>21</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J13" s="6">
         <v>139</v>
       </c>
-      <c r="J11" s="15">
+      <c r="K13" s="15">
         <v>180</v>
       </c>
-      <c r="K11" s="6">
+      <c r="L13" s="6">
         <v>3050</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M13" s="6">
         <v>1507</v>
       </c>
-      <c r="M11" s="6">
-        <v>25</v>
-      </c>
-      <c r="N11" s="11" t="s">
+      <c r="N13" s="6">
+        <v>25</v>
+      </c>
+      <c r="O13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="P13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="14">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5">
-        <v>16</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5">
-        <v>18</v>
-      </c>
-      <c r="I12" s="5">
-        <v>123</v>
-      </c>
-      <c r="J12" s="14">
-        <v>157</v>
-      </c>
-      <c r="K12" s="5">
-        <v>2890</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1517</v>
-      </c>
-      <c r="M12" s="5">
-        <v>25</v>
-      </c>
-      <c r="N12" s="10" t="s">
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="18">
         <v>5</v>
       </c>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="18">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="14">
-        <v>157</v>
-      </c>
-      <c r="K13" s="5">
-        <v>2840</v>
-      </c>
-      <c r="L13" s="5">
-        <v>1517</v>
-      </c>
-      <c r="M13" s="5">
-        <v>25</v>
-      </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="14">
-        <v>13</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9">
-        <v>34</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="5">
-        <v>32</v>
-      </c>
-      <c r="I14" s="5">
-        <v>168</v>
-      </c>
-      <c r="J14" s="14">
-        <v>234</v>
-      </c>
-      <c r="K14" s="5">
-        <v>3300</v>
-      </c>
-      <c r="L14" s="5">
-        <v>1617</v>
-      </c>
-      <c r="M14" s="5">
-        <v>35</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E14" s="22"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="15">
+        <v>150</v>
+      </c>
+      <c r="L14" s="6">
+        <v>2780</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1457</v>
+      </c>
+      <c r="N14" s="6">
+        <v>25</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="15">
-        <v>14</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="18">
+        <v>5</v>
+      </c>
+      <c r="E15" s="31"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6">
-        <v>36</v>
-      </c>
-      <c r="I15" s="6">
-        <v>108</v>
-      </c>
-      <c r="J15" s="15">
-        <v>160</v>
-      </c>
-      <c r="K15" s="6">
-        <v>3010</v>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="15">
+        <v>180</v>
       </c>
       <c r="L15" s="6">
-        <v>1407</v>
+        <v>2780</v>
       </c>
       <c r="M15" s="6">
-        <v>25</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="O15" s="20"/>
-    </row>
-    <row r="16" spans="1:15" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>1457</v>
+      </c>
+      <c r="N15" s="6">
+        <v>25</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="14">
         <v>11</v>
       </c>
-      <c r="C16" s="21">
+      <c r="E16" s="26"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5">
+        <v>16</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5">
+        <v>18</v>
+      </c>
+      <c r="J16" s="5">
+        <v>123</v>
+      </c>
+      <c r="K16" s="14">
+        <v>157</v>
+      </c>
+      <c r="L16" s="5">
+        <v>2890</v>
+      </c>
+      <c r="M16" s="5">
+        <v>1517</v>
+      </c>
+      <c r="N16" s="5">
+        <v>25</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="18">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="14">
+        <v>157</v>
+      </c>
+      <c r="L17" s="5">
+        <v>2840</v>
+      </c>
+      <c r="M17" s="5">
+        <v>1517</v>
+      </c>
+      <c r="N17" s="5">
+        <v>25</v>
+      </c>
+      <c r="O17" s="10"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="14">
+        <v>13</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9">
+        <v>34</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="5">
+        <v>32</v>
+      </c>
+      <c r="J18" s="5">
+        <v>168</v>
+      </c>
+      <c r="K18" s="14">
+        <v>234</v>
+      </c>
+      <c r="L18" s="5">
+        <v>3300</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1617</v>
+      </c>
+      <c r="N18" s="5">
+        <v>35</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="15">
+        <v>14</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6">
+        <v>16</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6">
+        <v>36</v>
+      </c>
+      <c r="J19" s="6">
+        <v>108</v>
+      </c>
+      <c r="K19" s="15">
+        <v>160</v>
+      </c>
+      <c r="L19" s="6">
+        <v>3010</v>
+      </c>
+      <c r="M19" s="6">
+        <v>1407</v>
+      </c>
+      <c r="N19" s="6">
+        <v>25</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="20"/>
+    </row>
+    <row r="20" spans="1:16" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="28">
         <v>15</v>
       </c>
-      <c r="D16" s="22">
+      <c r="E20" s="29">
         <v>29</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9">
+      <c r="F20" s="30"/>
+      <c r="G20" s="30">
         <v>20</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9">
+      <c r="H20" s="30"/>
+      <c r="I20" s="30">
         <v>21</v>
       </c>
-      <c r="I16" s="9">
+      <c r="J20" s="30">
         <v>139</v>
       </c>
-      <c r="J16" s="21">
+      <c r="K20" s="21">
         <v>180</v>
       </c>
-      <c r="K16" s="9">
+      <c r="L20" s="9">
         <v>3050</v>
       </c>
-      <c r="L16" s="9">
+      <c r="M20" s="9">
         <v>1407</v>
       </c>
-      <c r="M16" s="9">
-        <v>25</v>
-      </c>
-      <c r="N16" s="23" t="s">
+      <c r="N20" s="9">
+        <v>25</v>
+      </c>
+      <c r="O20" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="24" t="s">
+      <c r="P20" s="24" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="21">
+        <v>5</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="27">
+        <v>150</v>
+      </c>
+      <c r="L21" s="6">
+        <v>2780</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1457</v>
+      </c>
+      <c r="N21" s="6">
+        <v>25</v>
+      </c>
+      <c r="O21" s="11"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="16">
+        <v>5</v>
+      </c>
+      <c r="K22" s="21">
+        <v>180</v>
+      </c>
+      <c r="L22" s="6">
+        <v>2780</v>
+      </c>
+      <c r="M22" s="6">
+        <v>1457</v>
+      </c>
+      <c r="N22" s="7">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" tooltip="Airbus A320-200" display="https://en.wikipedia.org/wiki/Airbus_A320-200" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="N2" r:id="rId2" location="cite_note-35" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-35" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" tooltip="Airbus A330-200" display="https://en.wikipedia.org/wiki/Airbus_A330-200" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="N4" r:id="rId4" location="cite_note-40" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-40" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="O4" r:id="rId5" location="cite_note-PSRetrofit-41" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-PSRetrofit-41" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B5" r:id="rId6" tooltip="Boeing 737-800" display="https://en.wikipedia.org/wiki/Boeing_737-800" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="N5" r:id="rId7" location="cite_note-51" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-51" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B6" r:id="rId8" tooltip="Boeing 737-900ER" display="https://en.wikipedia.org/wiki/Boeing_737-900ER" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="N6" r:id="rId9" location="cite_note-52" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-52" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B7" r:id="rId10" tooltip="Airbus A320-200" display="https://en.wikipedia.org/wiki/Airbus_A320-200" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="N7" r:id="rId11" location="cite_note-35" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-35" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B9" r:id="rId12" tooltip="Airbus A330-200" display="https://en.wikipedia.org/wiki/Airbus_A330-200" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="N9" r:id="rId13" location="cite_note-40" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-40" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="O9" r:id="rId14" location="cite_note-PSRetrofit-41" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-PSRetrofit-41" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B10" r:id="rId15" tooltip="Boeing 737-800" display="https://en.wikipedia.org/wiki/Boeing_737-800" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="N10" r:id="rId16" location="cite_note-51" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-51" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B11" r:id="rId17" tooltip="Boeing 737-900ER" display="https://en.wikipedia.org/wiki/Boeing_737-900ER" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="N11" r:id="rId18" location="cite_note-52" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-52" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B12" r:id="rId19" tooltip="Airbus A320-200" display="https://en.wikipedia.org/wiki/Airbus_A320-200" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="N12" r:id="rId20" location="cite_note-35" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-35" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B14" r:id="rId21" tooltip="Airbus A330-200" display="https://en.wikipedia.org/wiki/Airbus_A330-200" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="N14" r:id="rId22" location="cite_note-40" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-40" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="O14" r:id="rId23" location="cite_note-PSRetrofit-41" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-PSRetrofit-41" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B15" r:id="rId24" tooltip="Boeing 737-800" display="https://en.wikipedia.org/wiki/Boeing_737-800" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="N15" r:id="rId25" location="cite_note-51" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-51" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B16" r:id="rId26" tooltip="Boeing 737-900ER" display="https://en.wikipedia.org/wiki/Boeing_737-900ER" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="N16" r:id="rId27" location="cite_note-52" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-52" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C2" r:id="rId1" tooltip="Airbus A320-200" display="https://en.wikipedia.org/wiki/Airbus_A320-200" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O2" r:id="rId2" location="cite_note-35" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-35" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" tooltip="Airbus A330-200" display="https://en.wikipedia.org/wiki/Airbus_A330-200" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="O4" r:id="rId4" location="cite_note-40" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-40" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="P4" r:id="rId5" location="cite_note-PSRetrofit-41" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-PSRetrofit-41" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C5" r:id="rId6" tooltip="Boeing 737-800" display="https://en.wikipedia.org/wiki/Boeing_737-800" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="O5" r:id="rId7" location="cite_note-51" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-51" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C6" r:id="rId8" tooltip="Boeing 737-900ER" display="https://en.wikipedia.org/wiki/Boeing_737-900ER" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="O6" r:id="rId9" location="cite_note-52" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-52" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C9" r:id="rId10" tooltip="Airbus A320-200" display="https://en.wikipedia.org/wiki/Airbus_A320-200" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="O9" r:id="rId11" location="cite_note-35" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-35" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C11" r:id="rId12" tooltip="Airbus A330-200" display="https://en.wikipedia.org/wiki/Airbus_A330-200" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="O11" r:id="rId13" location="cite_note-40" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-40" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="P11" r:id="rId14" location="cite_note-PSRetrofit-41" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-PSRetrofit-41" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C12" r:id="rId15" tooltip="Boeing 737-800" display="https://en.wikipedia.org/wiki/Boeing_737-800" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="O12" r:id="rId16" location="cite_note-51" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-51" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C13" r:id="rId17" tooltip="Boeing 737-900ER" display="https://en.wikipedia.org/wiki/Boeing_737-900ER" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="O13" r:id="rId18" location="cite_note-52" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-52" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C16" r:id="rId19" tooltip="Airbus A320-200" display="https://en.wikipedia.org/wiki/Airbus_A320-200" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="O16" r:id="rId20" location="cite_note-35" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-35" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C18" r:id="rId21" tooltip="Airbus A330-200" display="https://en.wikipedia.org/wiki/Airbus_A330-200" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="O18" r:id="rId22" location="cite_note-40" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-40" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="P18" r:id="rId23" location="cite_note-PSRetrofit-41" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-PSRetrofit-41" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C19" r:id="rId24" tooltip="Boeing 737-800" display="https://en.wikipedia.org/wiki/Boeing_737-800" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="O19" r:id="rId25" location="cite_note-51" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-51" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C20" r:id="rId26" tooltip="Boeing 737-900ER" display="https://en.wikipedia.org/wiki/Boeing_737-900ER" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="O20" r:id="rId27" location="cite_note-52" display="https://en.wikipedia.org/wiki/Delta_Air_Lines_fleet - cite_note-52" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>

</xml_diff>